<commit_message>
I worked out most of the errors that came with coupling the Unit Converter with this program. I also added a thermo table lookup.
</commit_message>
<xml_diff>
--- a/source/logic/thermoTable.xlsx
+++ b/source/logic/thermoTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="7635" windowHeight="1125" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="7635" windowHeight="1185" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
   <si>
     <t>Molar mass, gas constant, and critical-point properties</t>
   </si>
@@ -202,12 +202,6 @@
     <t>Temp</t>
   </si>
   <si>
-    <t>Sat. liquid</t>
-  </si>
-  <si>
-    <t>Sat. press</t>
-  </si>
-  <si>
     <t>Psat</t>
   </si>
   <si>
@@ -217,9 +211,6 @@
     <t>kPa</t>
   </si>
   <si>
-    <t>Sat.vapor</t>
-  </si>
-  <si>
     <t>Specific volume</t>
   </si>
   <si>
@@ -232,9 +223,6 @@
     <t>Entropy</t>
   </si>
   <si>
-    <t>Evap</t>
-  </si>
-  <si>
     <t>vg</t>
   </si>
   <si>
@@ -272,6 +260,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Liquid</t>
   </si>
 </sst>
 </file>
@@ -613,7 +604,7 @@
   <dimension ref="A1:G38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1366,7 +1357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1692,7 +1685,7 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2935,563 +2928,528 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M15"/>
+  <dimension ref="A1:N14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:M15"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="C2" t="s">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="D2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" t="s">
         <v>67</v>
       </c>
-      <c r="E2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H2" t="s">
-        <v>69</v>
-      </c>
-      <c r="K2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
         <v>60</v>
-      </c>
-      <c r="B3" t="s">
-        <v>62</v>
       </c>
       <c r="C3" t="s">
         <v>61</v>
       </c>
       <c r="D3" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>68</v>
       </c>
       <c r="F3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G3" t="s">
+        <v>70</v>
+      </c>
+      <c r="H3" t="s">
         <v>71</v>
       </c>
-      <c r="G3" t="s">
-        <v>66</v>
-      </c>
-      <c r="H3" t="s">
-        <v>61</v>
-      </c>
       <c r="I3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="J3" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="K3" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="L3" t="s">
-        <v>71</v>
+        <v>75</v>
       </c>
       <c r="M3" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>60</v>
-      </c>
+        <v>76</v>
+      </c>
+      <c r="N3" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
+        <v>80</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
       <c r="D4" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="E4" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="F4" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="G4" t="s">
-        <v>75</v>
+        <v>79</v>
       </c>
       <c r="H4" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="I4" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K4" t="s">
         <v>79</v>
       </c>
       <c r="L4" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="M4" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="N4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B5" t="s">
-        <v>65</v>
-      </c>
-      <c r="C5" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" t="s">
-        <v>82</v>
-      </c>
-      <c r="E5" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" t="s">
-        <v>83</v>
-      </c>
-      <c r="K5" t="s">
-        <v>7</v>
-      </c>
-      <c r="L5" t="s">
-        <v>7</v>
-      </c>
-      <c r="M5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6">
+        <v>40</v>
+      </c>
+      <c r="B5">
         <v>0.01</v>
       </c>
+      <c r="C5">
+        <v>0.61170000000000002</v>
+      </c>
+      <c r="D5">
+        <v>1E-3</v>
+      </c>
+      <c r="E5">
+        <v>206</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>2374.9</v>
+      </c>
+      <c r="H5">
+        <v>2374.9</v>
+      </c>
+      <c r="I5">
+        <v>1E-3</v>
+      </c>
+      <c r="J5">
+        <v>2500.9</v>
+      </c>
+      <c r="K5">
+        <v>2500.9</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>9.1555999999999997</v>
+      </c>
+      <c r="N5">
+        <v>9.1555999999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6">
-        <v>0.61170000000000002</v>
+        <v>5</v>
       </c>
       <c r="C6">
+        <v>0.87250000000000005</v>
+      </c>
+      <c r="D6">
         <v>1E-3</v>
       </c>
-      <c r="D6">
-        <v>206</v>
-      </c>
       <c r="E6">
-        <v>0</v>
+        <v>147.03</v>
       </c>
       <c r="F6">
-        <v>2374.9</v>
+        <v>21.018999999999998</v>
       </c>
       <c r="G6">
-        <v>2374.9</v>
+        <v>2360.8000000000002</v>
       </c>
       <c r="H6">
+        <v>2381.8000000000002</v>
+      </c>
+      <c r="I6">
+        <v>21.02</v>
+      </c>
+      <c r="J6">
+        <v>2489.1</v>
+      </c>
+      <c r="K6">
+        <v>2510.1</v>
+      </c>
+      <c r="L6">
+        <v>7.6300000000000007E-2</v>
+      </c>
+      <c r="M6">
+        <v>8.9487000000000005</v>
+      </c>
+      <c r="N6">
+        <v>9.0249000000000006</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>10</v>
+      </c>
+      <c r="C7">
+        <v>1.2281</v>
+      </c>
+      <c r="D7">
         <v>1E-3</v>
       </c>
-      <c r="I6">
-        <v>2500.9</v>
-      </c>
-      <c r="J6">
-        <v>2500.9</v>
-      </c>
-      <c r="K6">
-        <v>0</v>
-      </c>
-      <c r="L6">
-        <v>9.1555999999999997</v>
-      </c>
-      <c r="M6">
-        <v>9.1555999999999997</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>0.87250000000000005</v>
-      </c>
-      <c r="C7">
-        <v>1E-3</v>
-      </c>
-      <c r="D7">
-        <v>147.03</v>
-      </c>
       <c r="E7">
-        <v>21.018999999999998</v>
+        <v>106.32</v>
       </c>
       <c r="F7">
-        <v>2360.8000000000002</v>
+        <v>42.02</v>
       </c>
       <c r="G7">
-        <v>2381.8000000000002</v>
+        <v>2346.6</v>
       </c>
       <c r="H7">
-        <v>21.02</v>
+        <v>2388.6999999999998</v>
       </c>
       <c r="I7">
-        <v>2489.1</v>
+        <v>42.021999999999998</v>
       </c>
       <c r="J7">
-        <v>2510.1</v>
+        <v>2477.1999999999998</v>
       </c>
       <c r="K7">
-        <v>7.6300000000000007E-2</v>
+        <v>2519.1999999999998</v>
       </c>
       <c r="L7">
-        <v>8.9487000000000005</v>
+        <v>0.15110000000000001</v>
       </c>
       <c r="M7">
-        <v>9.0249000000000006</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <v>10</v>
-      </c>
+        <v>8.7487999999999992</v>
+      </c>
+      <c r="N7">
+        <v>8.8999000000000006</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>1.2281</v>
+        <v>15</v>
       </c>
       <c r="C8">
-        <v>1E-3</v>
+        <v>1.7057</v>
       </c>
       <c r="D8">
-        <v>106.32</v>
+        <v>1.0009999999999999E-3</v>
       </c>
       <c r="E8">
-        <v>42.02</v>
+        <v>77.885000000000005</v>
       </c>
       <c r="F8">
-        <v>2346.6</v>
+        <v>62.98</v>
       </c>
       <c r="G8">
-        <v>2388.6999999999998</v>
+        <v>2332.5</v>
       </c>
       <c r="H8">
-        <v>42.021999999999998</v>
+        <v>2395.5</v>
       </c>
       <c r="I8">
-        <v>2477.1999999999998</v>
+        <v>62.981999999999999</v>
       </c>
       <c r="J8">
-        <v>2519.1999999999998</v>
+        <v>2465.4</v>
       </c>
       <c r="K8">
-        <v>0.15110000000000001</v>
+        <v>2528.3000000000002</v>
       </c>
       <c r="L8">
-        <v>8.7487999999999992</v>
+        <v>0.22450000000000001</v>
       </c>
       <c r="M8">
-        <v>8.8999000000000006</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <v>15</v>
-      </c>
+        <v>8.5558999999999994</v>
+      </c>
+      <c r="N8">
+        <v>8.7803000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9">
-        <v>1.7057</v>
+        <v>20</v>
       </c>
       <c r="C9">
-        <v>1.0009999999999999E-3</v>
+        <v>2.3391999999999999</v>
       </c>
       <c r="D9">
-        <v>77.885000000000005</v>
+        <v>1.0020000000000001E-3</v>
       </c>
       <c r="E9">
-        <v>62.98</v>
+        <v>57.762</v>
       </c>
       <c r="F9">
-        <v>2332.5</v>
+        <v>83.912999999999997</v>
       </c>
       <c r="G9">
-        <v>2395.5</v>
+        <v>2318.4</v>
       </c>
       <c r="H9">
-        <v>62.981999999999999</v>
+        <v>2402.3000000000002</v>
       </c>
       <c r="I9">
-        <v>2465.4</v>
+        <v>83.915000000000006</v>
       </c>
       <c r="J9">
-        <v>2528.3000000000002</v>
+        <v>2453.5</v>
       </c>
       <c r="K9">
-        <v>0.22450000000000001</v>
+        <v>2537.4</v>
       </c>
       <c r="L9">
-        <v>8.5558999999999994</v>
+        <v>0.29649999999999999</v>
       </c>
       <c r="M9">
-        <v>8.7803000000000004</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <v>20</v>
-      </c>
+        <v>8.3696000000000002</v>
+      </c>
+      <c r="N9">
+        <v>8.6661000000000001</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10">
-        <v>2.3391999999999999</v>
+        <v>25</v>
       </c>
       <c r="C10">
-        <v>1.0020000000000001E-3</v>
+        <v>3.1698</v>
       </c>
       <c r="D10">
-        <v>57.762</v>
+        <v>1.003E-3</v>
       </c>
       <c r="E10">
-        <v>83.912999999999997</v>
+        <v>43.34</v>
       </c>
       <c r="F10">
-        <v>2318.4</v>
+        <v>104.83</v>
       </c>
       <c r="G10">
-        <v>2402.3000000000002</v>
+        <v>2304.3000000000002</v>
       </c>
       <c r="H10">
-        <v>83.915000000000006</v>
+        <v>2409.1</v>
       </c>
       <c r="I10">
-        <v>2453.5</v>
+        <v>104.83</v>
       </c>
       <c r="J10">
-        <v>2537.4</v>
+        <v>2441.6999999999998</v>
       </c>
       <c r="K10">
-        <v>0.29649999999999999</v>
+        <v>2546.5</v>
       </c>
       <c r="L10">
-        <v>8.3696000000000002</v>
+        <v>0.36720000000000003</v>
       </c>
       <c r="M10">
-        <v>8.6661000000000001</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <v>25</v>
-      </c>
+        <v>8.1895000000000007</v>
+      </c>
+      <c r="N10">
+        <v>8.5566999999999993</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11">
-        <v>3.1698</v>
+        <v>30</v>
       </c>
       <c r="C11">
-        <v>1.003E-3</v>
+        <v>4.2469000000000001</v>
       </c>
       <c r="D11">
-        <v>43.34</v>
+        <v>1.0039999999999999E-3</v>
       </c>
       <c r="E11">
-        <v>104.83</v>
+        <v>32.878999999999998</v>
       </c>
       <c r="F11">
-        <v>2304.3000000000002</v>
+        <v>125.73</v>
       </c>
       <c r="G11">
-        <v>2409.1</v>
+        <v>2290.1999999999998</v>
       </c>
       <c r="H11">
-        <v>104.83</v>
+        <v>2415.9</v>
       </c>
       <c r="I11">
-        <v>2441.6999999999998</v>
+        <v>125.74</v>
       </c>
       <c r="J11">
-        <v>2546.5</v>
+        <v>2429.8000000000002</v>
       </c>
       <c r="K11">
-        <v>0.36720000000000003</v>
+        <v>2555.6</v>
       </c>
       <c r="L11">
-        <v>8.1895000000000007</v>
+        <v>0.43680000000000002</v>
       </c>
       <c r="M11">
-        <v>8.5566999999999993</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <v>30</v>
-      </c>
+        <v>8.0152000000000001</v>
+      </c>
+      <c r="N11">
+        <v>8.452</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12">
-        <v>4.2469000000000001</v>
+        <v>35</v>
       </c>
       <c r="C12">
-        <v>1.0039999999999999E-3</v>
+        <v>5.6291000000000002</v>
       </c>
       <c r="D12">
-        <v>32.878999999999998</v>
+        <v>1.0059999999999999E-3</v>
       </c>
       <c r="E12">
-        <v>125.73</v>
+        <v>25.204999999999998</v>
       </c>
       <c r="F12">
-        <v>2290.1999999999998</v>
+        <v>146.63</v>
       </c>
       <c r="G12">
-        <v>2415.9</v>
+        <v>2276</v>
       </c>
       <c r="H12">
-        <v>125.74</v>
+        <v>2422.6999999999998</v>
       </c>
       <c r="I12">
-        <v>2429.8000000000002</v>
+        <v>146.63999999999999</v>
       </c>
       <c r="J12">
-        <v>2555.6</v>
+        <v>2417.9</v>
       </c>
       <c r="K12">
-        <v>0.43680000000000002</v>
+        <v>2564.6</v>
       </c>
       <c r="L12">
-        <v>8.0152000000000001</v>
+        <v>0.50509999999999999</v>
       </c>
       <c r="M12">
-        <v>8.452</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <v>35</v>
-      </c>
+        <v>7.8465999999999996</v>
+      </c>
+      <c r="N12">
+        <v>8.3516999999999992</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
-        <v>5.6291000000000002</v>
+        <v>40</v>
       </c>
       <c r="C13">
-        <v>1.0059999999999999E-3</v>
+        <v>7.3851000000000004</v>
       </c>
       <c r="D13">
-        <v>25.204999999999998</v>
+        <v>1.008E-3</v>
       </c>
       <c r="E13">
-        <v>146.63</v>
+        <v>19.515000000000001</v>
       </c>
       <c r="F13">
-        <v>2276</v>
+        <v>167.53</v>
       </c>
       <c r="G13">
-        <v>2422.6999999999998</v>
+        <v>2261.9</v>
       </c>
       <c r="H13">
-        <v>146.63999999999999</v>
+        <v>2429.4</v>
       </c>
       <c r="I13">
-        <v>2417.9</v>
+        <v>167.53</v>
       </c>
       <c r="J13">
-        <v>2564.6</v>
+        <v>2406</v>
       </c>
       <c r="K13">
-        <v>0.50509999999999999</v>
+        <v>2573.5</v>
       </c>
       <c r="L13">
-        <v>7.8465999999999996</v>
+        <v>0.57240000000000002</v>
       </c>
       <c r="M13">
-        <v>8.3516999999999992</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14">
-        <v>40</v>
-      </c>
+        <v>7.6832000000000003</v>
+      </c>
+      <c r="N13">
+        <v>8.2555999999999994</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
-        <v>7.3851000000000004</v>
+        <v>45</v>
       </c>
       <c r="C14">
-        <v>1.008E-3</v>
+        <v>9.5952999999999999</v>
       </c>
       <c r="D14">
-        <v>19.515000000000001</v>
+        <v>1.01E-3</v>
       </c>
       <c r="E14">
-        <v>167.53</v>
+        <v>15.250999999999999</v>
       </c>
       <c r="F14">
-        <v>2261.9</v>
+        <v>188.43</v>
       </c>
       <c r="G14">
-        <v>2429.4</v>
+        <v>2247.6999999999998</v>
       </c>
       <c r="H14">
-        <v>167.53</v>
+        <v>2436.1</v>
       </c>
       <c r="I14">
-        <v>2406</v>
+        <v>188.44</v>
       </c>
       <c r="J14">
-        <v>2573.5</v>
+        <v>2394</v>
       </c>
       <c r="K14">
-        <v>0.57240000000000002</v>
+        <v>2582.4</v>
       </c>
       <c r="L14">
-        <v>7.6832000000000003</v>
+        <v>0.63859999999999995</v>
       </c>
       <c r="M14">
-        <v>8.2555999999999994</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>45</v>
-      </c>
-      <c r="B15">
-        <v>9.5952999999999999</v>
-      </c>
-      <c r="C15">
-        <v>1.01E-3</v>
-      </c>
-      <c r="D15">
-        <v>15.250999999999999</v>
-      </c>
-      <c r="E15">
-        <v>188.43</v>
-      </c>
-      <c r="F15">
-        <v>2247.6999999999998</v>
-      </c>
-      <c r="G15">
-        <v>2436.1</v>
-      </c>
-      <c r="H15">
-        <v>188.44</v>
-      </c>
-      <c r="I15">
-        <v>2394</v>
-      </c>
-      <c r="J15">
-        <v>2582.4</v>
-      </c>
-      <c r="K15">
-        <v>0.63859999999999995</v>
-      </c>
-      <c r="L15">
         <v>7.5247000000000002</v>
       </c>
-      <c r="M15">
+      <c r="N14">
         <v>8.1632999999999996</v>
       </c>
     </row>

</xml_diff>

<commit_message>
The program is almost done. The Numerical methood still needs a bit of work.
</commit_message>
<xml_diff>
--- a/source/logic/thermoTable.xlsx
+++ b/source/logic/thermoTable.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="0" windowWidth="7635" windowHeight="1185" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="0" windowWidth="7635" windowHeight="1185"/>
   </bookViews>
   <sheets>
     <sheet name="A1" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="83">
   <si>
     <t>Molar mass, gas constant, and critical-point properties</t>
   </si>
@@ -148,12 +148,6 @@
     <t>Temperature</t>
   </si>
   <si>
-    <t>Pressure</t>
-  </si>
-  <si>
-    <t>Volume</t>
-  </si>
-  <si>
     <t>K</t>
   </si>
   <si>
@@ -263,6 +257,15 @@
   </si>
   <si>
     <t>Liquid</t>
+  </si>
+  <si>
+    <t>Critical Temperature</t>
+  </si>
+  <si>
+    <t>Critical Pressure</t>
+  </si>
+  <si>
+    <t>Critical Volume</t>
   </si>
 </sst>
 </file>
@@ -603,8 +606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I3" sqref="I3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -622,7 +625,7 @@
         <v>0</v>
       </c>
       <c r="E1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -639,13 +642,13 @@
         <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>42</v>
+        <v>80</v>
       </c>
       <c r="F3" t="s">
-        <v>43</v>
+        <v>81</v>
       </c>
       <c r="G3" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -656,13 +659,13 @@
         <v>7</v>
       </c>
       <c r="E4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G4" t="s">
         <v>45</v>
-      </c>
-      <c r="F4" t="s">
-        <v>46</v>
-      </c>
-      <c r="G4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1369,12 +1372,12 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>2</v>
@@ -1383,18 +1386,18 @@
         <v>4</v>
       </c>
       <c r="D3" t="s">
+        <v>49</v>
+      </c>
+      <c r="E3" t="s">
+        <v>50</v>
+      </c>
+      <c r="F3" t="s">
         <v>51</v>
-      </c>
-      <c r="E3" t="s">
-        <v>52</v>
-      </c>
-      <c r="F3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D4" t="s">
         <v>7</v>
@@ -1439,7 +1442,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C7">
         <v>0.14330000000000001</v>
@@ -1609,7 +1612,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C17">
         <v>7.2900000000000006E-2</v>
@@ -1660,7 +1663,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C20">
         <v>0.46150000000000002</v>
@@ -1685,7 +1688,7 @@
   <dimension ref="A1:E93"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1696,29 +1699,29 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B3" t="s">
         <v>42</v>
       </c>
       <c r="C3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" t="s">
         <v>51</v>
-      </c>
-      <c r="D3" t="s">
-        <v>52</v>
-      </c>
-      <c r="E3" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
         <v>7</v>
@@ -2930,105 +2933,105 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" t="s">
         <v>64</v>
       </c>
-      <c r="F2" t="s">
+      <c r="L2" t="s">
         <v>65</v>
-      </c>
-      <c r="I2" t="s">
-        <v>66</v>
-      </c>
-      <c r="L2" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
         <v>60</v>
       </c>
-      <c r="C3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D3" t="s">
-        <v>62</v>
-      </c>
       <c r="E3" t="s">
+        <v>66</v>
+      </c>
+      <c r="F3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" t="s">
         <v>68</v>
       </c>
-      <c r="F3" t="s">
+      <c r="H3" t="s">
         <v>69</v>
       </c>
-      <c r="G3" t="s">
+      <c r="I3" t="s">
         <v>70</v>
       </c>
-      <c r="H3" t="s">
+      <c r="J3" t="s">
         <v>71</v>
       </c>
-      <c r="I3" t="s">
+      <c r="K3" t="s">
         <v>72</v>
       </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
         <v>73</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>74</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>75</v>
-      </c>
-      <c r="M3" t="s">
-        <v>76</v>
-      </c>
-      <c r="N3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="J4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="K4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="L4" t="s">
         <v>7</v>

</xml_diff>